<commit_message>
fix: fix age_adjusted rates calc. on tables
</commit_message>
<xml_diff>
--- a/tables/table_overview.xlsx
+++ b/tables/table_overview.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Analise</t>
   </si>
@@ -89,16 +89,65 @@
   </si>
   <si>
     <t xml:space="preserve">Deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_Yellow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_Indigenous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_NoInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_Public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_Private</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths_ONG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-409]#,##0"/>
-    <numFmt numFmtId="166" formatCode="[$-409]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="[$-409]General"/>
+    <numFmt numFmtId="167" formatCode="[$-409]#,##0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -180,8 +229,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -189,11 +242,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -214,852 +267,1663 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16:N18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S20" activeCellId="0" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="2" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="1" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="C1" s="3" t="n">
         <v>2011</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="D1" s="3" t="n">
         <v>2012</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="E1" s="3" t="n">
         <v>2013</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="F1" s="3" t="n">
         <v>2014</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="G1" s="3" t="n">
         <v>2015</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="H1" s="3" t="n">
         <v>2016</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="I1" s="3" t="n">
         <v>2017</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="J1" s="3" t="n">
         <v>2018</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="K1" s="3" t="n">
         <v>2019</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="C2" s="1" t="n">
         <v>362159</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="D2" s="1" t="n">
         <v>344545</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="E2" s="1" t="n">
         <v>359744</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="F2" s="1" t="n">
         <v>344402</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="G2" s="1" t="n">
         <v>339809</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="H2" s="1" t="n">
         <v>338561</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="I2" s="1" t="n">
         <v>351769</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="J2" s="1" t="n">
         <v>349995</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="K2" s="1" t="n">
         <v>353591</v>
       </c>
-      <c r="K2" s="3" t="n">
+      <c r="L2" s="4" t="n">
         <v>-2.36581170149023</v>
       </c>
-      <c r="L2" s="3" t="n">
+      <c r="M2" s="4" t="n">
         <v>-0.189257385313579</v>
       </c>
-      <c r="M2" s="3" t="n">
+      <c r="N2" s="4" t="n">
         <v>-0.231974338823937</v>
       </c>
-      <c r="N2" s="3" t="n">
+      <c r="O2" s="4" t="n">
         <v>-0.146522141994376</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="C3" s="1" t="n">
         <v>182867</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="D3" s="1" t="n">
         <v>172784</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="E3" s="1" t="n">
         <v>180275</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="F3" s="1" t="n">
         <v>171844</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="G3" s="1" t="n">
         <v>169033</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="H3" s="1" t="n">
         <v>169297</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="I3" s="1" t="n">
         <v>173313</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="J3" s="1" t="n">
         <v>173638</v>
       </c>
-      <c r="J3" s="2" t="n">
+      <c r="K3" s="1" t="n">
         <v>174880</v>
       </c>
-      <c r="K3" s="3" t="n">
+      <c r="L3" s="4" t="n">
         <v>-4.36765518108789</v>
       </c>
-      <c r="L3" s="3" t="n">
+      <c r="M3" s="4" t="n">
         <v>-0.437752936884994</v>
       </c>
-      <c r="M3" s="3" t="n">
+      <c r="N3" s="4" t="n">
         <v>-0.498093649390985</v>
       </c>
-      <c r="N3" s="3" t="n">
+      <c r="O3" s="4" t="n">
         <v>-0.377375632099308</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="C4" s="1" t="n">
         <v>179292</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="D4" s="1" t="n">
         <v>171761</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="E4" s="1" t="n">
         <v>179469</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="F4" s="1" t="n">
         <v>172558</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="G4" s="1" t="n">
         <v>170776</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="H4" s="1" t="n">
         <v>169264</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="I4" s="1" t="n">
         <v>178456</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="J4" s="1" t="n">
         <v>176357</v>
       </c>
-      <c r="J4" s="2" t="n">
+      <c r="K4" s="1" t="n">
         <v>178711</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="L4" s="4" t="n">
         <v>-0.324052383820806</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="M4" s="4" t="n">
         <v>0.0584703861980174</v>
       </c>
-      <c r="M4" s="3" t="n">
+      <c r="N4" s="4" t="n">
         <v>-0.00200098192610909</v>
       </c>
-      <c r="N4" s="3" t="n">
+      <c r="O4" s="4" t="n">
         <v>0.118978322917496</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="C5" s="1" t="n">
         <v>136488</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="D5" s="1" t="n">
         <v>127530</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="E5" s="1" t="n">
         <v>138214</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="F5" s="1" t="n">
         <v>131724</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="G5" s="1" t="n">
         <v>131292</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="H5" s="1" t="n">
         <v>140834</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="I5" s="1" t="n">
         <v>138045</v>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="J5" s="1" t="n">
         <v>137816</v>
       </c>
-      <c r="J5" s="2" t="n">
+      <c r="K5" s="1" t="n">
         <v>137658</v>
       </c>
-      <c r="K5" s="3" t="n">
+      <c r="L5" s="4" t="n">
         <v>0.857218216986109</v>
       </c>
-      <c r="L5" s="3" t="n">
+      <c r="M5" s="4" t="n">
         <v>0.546483238351159</v>
       </c>
-      <c r="M5" s="3" t="n">
+      <c r="N5" s="4" t="n">
         <v>0.477391057401455</v>
       </c>
-      <c r="N5" s="3" t="n">
+      <c r="O5" s="4" t="n">
         <v>0.615622929784743</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="C6" s="1" t="n">
         <v>11986</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="D6" s="1" t="n">
         <v>10829</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="E6" s="1" t="n">
         <v>10893</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="F6" s="1" t="n">
         <v>10711</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="G6" s="1" t="n">
         <v>10560</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="H6" s="1" t="n">
         <v>11447</v>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="I6" s="1" t="n">
         <v>12454</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="J6" s="1" t="n">
         <v>12605</v>
       </c>
-      <c r="J6" s="2" t="n">
+      <c r="K6" s="1" t="n">
         <v>13331</v>
       </c>
-      <c r="K6" s="3" t="n">
+      <c r="L6" s="4" t="n">
         <v>11.2214249958285</v>
       </c>
-      <c r="L6" s="3" t="n">
+      <c r="M6" s="4" t="n">
         <v>2.1076528021216</v>
       </c>
-      <c r="M6" s="3" t="n">
+      <c r="N6" s="4" t="n">
         <v>1.8683124924435</v>
       </c>
-      <c r="N6" s="3" t="n">
+      <c r="O6" s="4" t="n">
         <v>2.34755544352421</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="C7" s="1" t="n">
         <v>95244</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="D7" s="1" t="n">
         <v>91185</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="E7" s="1" t="n">
         <v>101326</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="F7" s="1" t="n">
         <v>101450</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="G7" s="1" t="n">
         <v>100352</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="H7" s="1" t="n">
         <v>93363</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="I7" s="1" t="n">
         <v>105470</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="J7" s="1" t="n">
         <v>109579</v>
       </c>
-      <c r="J7" s="2" t="n">
+      <c r="K7" s="1" t="n">
         <v>114226</v>
       </c>
-      <c r="K7" s="3" t="n">
+      <c r="L7" s="4" t="n">
         <v>19.9298643484104</v>
       </c>
-      <c r="L7" s="3" t="n">
+      <c r="M7" s="4" t="n">
         <v>2.18414673408938</v>
       </c>
-      <c r="M7" s="3" t="n">
+      <c r="N7" s="4" t="n">
         <v>2.10288687603644</v>
       </c>
-      <c r="N7" s="3" t="n">
+      <c r="O7" s="4" t="n">
         <v>2.26547126381549</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="C8" s="1" t="n">
         <v>1382</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="D8" s="1" t="n">
         <v>1452</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="E8" s="1" t="n">
         <v>1484</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="F8" s="1" t="n">
         <v>1643</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="G8" s="1" t="n">
         <v>3503</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="H8" s="1" t="n">
         <v>6738</v>
       </c>
-      <c r="H8" s="2" t="n">
+      <c r="I8" s="1" t="n">
         <v>9310</v>
       </c>
-      <c r="I8" s="2" t="n">
+      <c r="J8" s="1" t="n">
         <v>10917</v>
       </c>
-      <c r="J8" s="2" t="n">
+      <c r="K8" s="1" t="n">
         <v>11868</v>
       </c>
-      <c r="K8" s="3" t="n">
+      <c r="L8" s="4" t="n">
         <v>758.755426917511</v>
       </c>
-      <c r="L8" s="3" t="n">
+      <c r="M8" s="4" t="n">
         <v>37.7825280680369</v>
       </c>
-      <c r="M8" s="3" t="n">
+      <c r="N8" s="4" t="n">
         <v>37.2091660889516</v>
       </c>
-      <c r="N8" s="3" t="n">
+      <c r="O8" s="4" t="n">
         <v>38.3582859800502</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="C9" s="1" t="n">
         <v>749</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="D9" s="1" t="n">
         <v>582</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="E9" s="1" t="n">
         <v>681</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="F9" s="1" t="n">
         <v>704</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="G9" s="1" t="n">
         <v>665</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="H9" s="1" t="n">
         <v>702</v>
       </c>
-      <c r="H9" s="2" t="n">
+      <c r="I9" s="1" t="n">
         <v>824</v>
       </c>
-      <c r="I9" s="2" t="n">
+      <c r="J9" s="1" t="n">
         <v>919</v>
       </c>
-      <c r="J9" s="2" t="n">
+      <c r="K9" s="1" t="n">
         <v>1009</v>
       </c>
-      <c r="K9" s="3" t="n">
+      <c r="L9" s="4" t="n">
         <v>34.7129506008011</v>
       </c>
-      <c r="L9" s="3" t="n">
+      <c r="M9" s="4" t="n">
         <v>5.27739672666012</v>
       </c>
-      <c r="M9" s="3" t="n">
+      <c r="N9" s="4" t="n">
         <v>4.31000119129064</v>
       </c>
-      <c r="N9" s="3" t="n">
+      <c r="O9" s="4" t="n">
         <v>6.25376411622542</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="C10" s="1" t="n">
         <v>116310</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="D10" s="1" t="n">
         <v>112967</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="E10" s="1" t="n">
         <v>107146</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="F10" s="1" t="n">
         <v>98170</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="G10" s="1" t="n">
         <v>93437</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="H10" s="1" t="n">
         <v>85477</v>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="I10" s="1" t="n">
         <v>85666</v>
       </c>
-      <c r="I10" s="2" t="n">
+      <c r="J10" s="1" t="n">
         <v>78159</v>
       </c>
-      <c r="J10" s="2" t="n">
+      <c r="K10" s="1" t="n">
         <v>75499</v>
       </c>
-      <c r="K10" s="3" t="n">
+      <c r="L10" s="4" t="n">
         <v>-35.0881265583355</v>
       </c>
-      <c r="L10" s="3" t="n">
+      <c r="M10" s="4" t="n">
         <v>-5.55196123076878</v>
       </c>
-      <c r="M10" s="3" t="n">
+      <c r="N10" s="4" t="n">
         <v>-5.63008250827888</v>
       </c>
-      <c r="N10" s="3" t="n">
+      <c r="O10" s="4" t="n">
         <v>-5.47377528292556</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="C11" s="1" t="n">
         <v>84638</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="D11" s="1" t="n">
         <v>80327</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="E11" s="1" t="n">
         <v>84718</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="F11" s="1" t="n">
         <v>78494</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="G11" s="1" t="n">
         <v>78895</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="H11" s="1" t="n">
         <v>86906</v>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="I11" s="1" t="n">
         <v>83924</v>
       </c>
-      <c r="I11" s="2" t="n">
+      <c r="J11" s="1" t="n">
         <v>82880</v>
       </c>
-      <c r="J11" s="2" t="n">
+      <c r="K11" s="1" t="n">
         <v>80403</v>
       </c>
-      <c r="K11" s="3" t="n">
+      <c r="L11" s="4" t="n">
         <v>-5.00366265743519</v>
       </c>
-      <c r="L11" s="3" t="n">
+      <c r="M11" s="4" t="n">
         <v>-0.0497120840237453</v>
       </c>
-      <c r="M11" s="3" t="n">
+      <c r="N11" s="4" t="n">
         <v>-0.137801398088844</v>
       </c>
-      <c r="N11" s="3" t="n">
+      <c r="O11" s="4" t="n">
         <v>0.038454934391563</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="C12" s="1" t="n">
         <v>25683</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="D12" s="1" t="n">
         <v>25503</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="E12" s="1" t="n">
         <v>26474</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="F12" s="1" t="n">
         <v>25900</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="G12" s="1" t="n">
         <v>23595</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="H12" s="1" t="n">
         <v>20793</v>
       </c>
-      <c r="H12" s="2" t="n">
+      <c r="I12" s="1" t="n">
         <v>24965</v>
       </c>
-      <c r="I12" s="2" t="n">
+      <c r="J12" s="1" t="n">
         <v>25011</v>
       </c>
-      <c r="J12" s="2" t="n">
+      <c r="K12" s="1" t="n">
         <v>25231</v>
       </c>
-      <c r="K12" s="3" t="n">
+      <c r="L12" s="4" t="n">
         <v>-1.75991901257641</v>
       </c>
-      <c r="L12" s="3" t="n">
+      <c r="M12" s="4" t="n">
         <v>-0.764016574875359</v>
       </c>
-      <c r="M12" s="3" t="n">
+      <c r="N12" s="4" t="n">
         <v>-0.923370594242268</v>
       </c>
-      <c r="N12" s="3" t="n">
+      <c r="O12" s="4" t="n">
         <v>-0.604406251840861</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="C13" s="1" t="n">
         <v>85814</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="D13" s="1" t="n">
         <v>77000</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="E13" s="1" t="n">
         <v>81068</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="F13" s="1" t="n">
         <v>79515</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="G13" s="1" t="n">
         <v>81580</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="H13" s="1" t="n">
         <v>69061</v>
       </c>
-      <c r="H13" s="2" t="n">
+      <c r="I13" s="1" t="n">
         <v>81625</v>
       </c>
-      <c r="I13" s="2" t="n">
+      <c r="J13" s="1" t="n">
         <v>84532</v>
       </c>
-      <c r="J13" s="2" t="n">
+      <c r="K13" s="1" t="n">
         <v>86787</v>
       </c>
-      <c r="K13" s="3" t="n">
+      <c r="L13" s="4" t="n">
         <v>1.13384762393083</v>
       </c>
-      <c r="L13" s="3" t="n">
+      <c r="M13" s="4" t="n">
         <v>0.354451692324775</v>
       </c>
-      <c r="M13" s="3" t="n">
+      <c r="N13" s="4" t="n">
         <v>0.265144514624049</v>
       </c>
-      <c r="N13" s="3" t="n">
+      <c r="O13" s="4" t="n">
         <v>0.443838416831377</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="C14" s="1" t="n">
         <v>136663</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="D14" s="1" t="n">
         <v>133306</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="E14" s="1" t="n">
         <v>136724</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="F14" s="1" t="n">
         <v>131235</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="G14" s="1" t="n">
         <v>127786</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="H14" s="1" t="n">
         <v>134384</v>
       </c>
-      <c r="H14" s="2" t="n">
+      <c r="I14" s="1" t="n">
         <v>134129</v>
       </c>
-      <c r="I14" s="2" t="n">
+      <c r="J14" s="1" t="n">
         <v>131308</v>
       </c>
-      <c r="J14" s="2" t="n">
+      <c r="K14" s="1" t="n">
         <v>133712</v>
       </c>
-      <c r="K14" s="3" t="n">
+      <c r="L14" s="4" t="n">
         <v>-2.15932622582557</v>
       </c>
-      <c r="L14" s="3" t="n">
+      <c r="M14" s="4" t="n">
         <v>-0.247837672141948</v>
       </c>
-      <c r="M14" s="3" t="n">
+      <c r="N14" s="4" t="n">
         <v>-0.316959734526567</v>
       </c>
-      <c r="N14" s="3" t="n">
+      <c r="O14" s="4" t="n">
         <v>-0.178667679241795</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="C15" s="1" t="n">
         <v>29361</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="D15" s="1" t="n">
         <v>28409</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="E15" s="1" t="n">
         <v>30760</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="F15" s="1" t="n">
         <v>29258</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="G15" s="1" t="n">
         <v>27953</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="H15" s="1" t="n">
         <v>27417</v>
       </c>
-      <c r="H15" s="2" t="n">
+      <c r="I15" s="1" t="n">
         <v>27126</v>
       </c>
-      <c r="I15" s="2" t="n">
+      <c r="J15" s="1" t="n">
         <v>26264</v>
       </c>
-      <c r="J15" s="2" t="n">
+      <c r="K15" s="1" t="n">
         <v>27458</v>
       </c>
-      <c r="K15" s="3" t="n">
+      <c r="L15" s="4" t="n">
         <v>-6.48138687374408</v>
       </c>
-      <c r="L15" s="3" t="n">
+      <c r="M15" s="4" t="n">
         <v>-1.3584857655882</v>
       </c>
-      <c r="M15" s="3" t="n">
+      <c r="N15" s="4" t="n">
         <v>-1.50700094362094</v>
       </c>
-      <c r="N15" s="3" t="n">
+      <c r="O15" s="4" t="n">
         <v>-1.20974664516039</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="C16" s="1" t="n">
         <v>147871</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="D16" s="1" t="n">
         <v>139816</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="E16" s="1" t="n">
         <v>150154</v>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="F16" s="1" t="n">
         <v>143432</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="G16" s="1" t="n">
         <v>144173</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="H16" s="1" t="n">
         <v>136958</v>
       </c>
-      <c r="H16" s="2" t="n">
+      <c r="I16" s="1" t="n">
         <v>151321</v>
       </c>
-      <c r="I16" s="2" t="n">
+      <c r="J16" s="1" t="n">
         <v>155074</v>
       </c>
-      <c r="J16" s="2" t="n">
+      <c r="K16" s="1" t="n">
         <v>158033</v>
       </c>
-      <c r="K16" s="3" t="n">
+      <c r="L16" s="4" t="n">
         <v>6.87220617971069</v>
       </c>
-      <c r="L16" s="3" t="n">
+      <c r="M16" s="4" t="n">
         <v>0.934659129387594</v>
       </c>
-      <c r="M16" s="3" t="n">
+      <c r="N16" s="4" t="n">
         <v>0.868153257112381</v>
       </c>
-      <c r="N16" s="3" t="n">
+      <c r="O16" s="4" t="n">
         <v>1.00120885129131</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="C17" s="1" t="n">
         <v>27441</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="D17" s="1" t="n">
         <v>26817</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="E17" s="1" t="n">
         <v>26267</v>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="F17" s="1" t="n">
         <v>26158</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="G17" s="1" t="n">
         <v>25272</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="H17" s="1" t="n">
         <v>23180</v>
       </c>
-      <c r="H17" s="2" t="n">
+      <c r="I17" s="1" t="n">
         <v>23454</v>
       </c>
-      <c r="I17" s="2" t="n">
+      <c r="J17" s="1" t="n">
         <v>21995</v>
       </c>
-      <c r="J17" s="2" t="n">
+      <c r="K17" s="1" t="n">
         <v>22853</v>
       </c>
-      <c r="K17" s="3" t="n">
+      <c r="L17" s="4" t="n">
         <v>-16.719507306585</v>
       </c>
-      <c r="L17" s="3" t="n">
+      <c r="M17" s="4" t="n">
         <v>-2.74533889070945</v>
       </c>
-      <c r="M17" s="3" t="n">
+      <c r="N17" s="4" t="n">
         <v>-2.90164165696507</v>
       </c>
-      <c r="N17" s="3" t="n">
+      <c r="O17" s="4" t="n">
         <v>-2.58878451819439</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="C18" s="1" t="n">
         <v>157516</v>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="D18" s="1" t="n">
         <v>153824</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="E18" s="1" t="n">
         <v>164824</v>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="F18" s="1" t="n">
         <v>159497</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="G18" s="1" t="n">
         <v>157866</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="H18" s="1" t="n">
         <v>168774</v>
       </c>
-      <c r="H18" s="2" t="n">
+      <c r="I18" s="1" t="n">
         <v>170217</v>
       </c>
-      <c r="I18" s="2" t="n">
+      <c r="J18" s="1" t="n">
         <v>168894</v>
       </c>
-      <c r="J18" s="2" t="n">
+      <c r="K18" s="1" t="n">
         <v>169922</v>
       </c>
-      <c r="K18" s="3" t="n">
+      <c r="L18" s="4" t="n">
         <v>7.87602529266868</v>
       </c>
-      <c r="L18" s="3" t="n">
+      <c r="M18" s="4" t="n">
         <v>1.17846491763076</v>
       </c>
-      <c r="M18" s="3" t="n">
+      <c r="N18" s="4" t="n">
         <v>1.11514906963481</v>
       </c>
-      <c r="N18" s="3" t="n">
+      <c r="O18" s="4" t="n">
         <v>1.24182041247134</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="C19" s="1" t="n">
         <v>43615</v>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="D19" s="1" t="n">
         <v>45225</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="E19" s="1" t="n">
         <v>49196</v>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="F19" s="1" t="n">
         <v>49246</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="G19" s="1" t="n">
         <v>52225</v>
       </c>
-      <c r="G19" s="2" t="n">
+      <c r="H19" s="1" t="n">
         <v>55595</v>
       </c>
-      <c r="H19" s="2" t="n">
+      <c r="I19" s="1" t="n">
         <v>55836</v>
       </c>
-      <c r="I19" s="2" t="n">
+      <c r="J19" s="1" t="n">
         <v>57379</v>
       </c>
-      <c r="J19" s="2" t="n">
+      <c r="K19" s="1" t="n">
         <v>59337</v>
       </c>
-      <c r="K19" s="3" t="n">
+      <c r="L19" s="4" t="n">
         <v>36.0472314570675</v>
       </c>
-      <c r="L19" s="3" t="n">
+      <c r="M19" s="4" t="n">
         <v>3.89792159626812</v>
       </c>
-      <c r="M19" s="3" t="n">
+      <c r="N19" s="4" t="n">
         <v>3.78231140922245</v>
       </c>
-      <c r="N19" s="3" t="n">
+      <c r="O19" s="4" t="n">
         <v>4.01366056937731</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>23372</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>24036</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>26057</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>25779</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>26875</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>29135</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>28683</v>
+      </c>
+      <c r="J20" s="1" t="n">
+        <v>29929</v>
+      </c>
+      <c r="K20" s="1" t="n">
+        <v>30611</v>
+      </c>
+      <c r="L20" s="4" t="n">
+        <v>30.9729590963546</v>
+      </c>
+      <c r="M20" s="4" t="n">
+        <v>3.4530758060868</v>
+      </c>
+      <c r="N20" s="4" t="n">
+        <v>3.29399833630923</v>
+      </c>
+      <c r="O20" s="4" t="n">
+        <v>3.61239826242503</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>20243</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>21189</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>23139</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>23467</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>25350</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>26460</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>27153</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>27450</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>28726</v>
+      </c>
+      <c r="L21" s="4" t="n">
+        <v>41.9058439954552</v>
+      </c>
+      <c r="M21" s="4" t="n">
+        <v>4.3881118429183</v>
+      </c>
+      <c r="N21" s="4" t="n">
+        <v>4.21987994428232</v>
+      </c>
+      <c r="O21" s="4" t="n">
+        <v>4.55661530175691</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>18583</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>18389</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>20805</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>21436</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>23737</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>22966</v>
+      </c>
+      <c r="J22" s="1" t="n">
+        <v>23904</v>
+      </c>
+      <c r="K22" s="1" t="n">
+        <v>24582</v>
+      </c>
+      <c r="L22" s="4" t="n">
+        <v>32.2821934025722</v>
+      </c>
+      <c r="M22" s="4" t="n">
+        <v>3.75085322841335</v>
+      </c>
+      <c r="N22" s="4" t="n">
+        <v>3.57224514381658</v>
+      </c>
+      <c r="O22" s="4" t="n">
+        <v>3.92976931876821</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>1423</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>1372</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>1501</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>1564</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>1588</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>1821</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>2037</v>
+      </c>
+      <c r="J23" s="1" t="n">
+        <v>2208</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v>2446</v>
+      </c>
+      <c r="L23" s="4" t="n">
+        <v>71.890372452565</v>
+      </c>
+      <c r="M23" s="4" t="n">
+        <v>7.79845788147187</v>
+      </c>
+      <c r="N23" s="4" t="n">
+        <v>7.14523959149873</v>
+      </c>
+      <c r="O23" s="4" t="n">
+        <v>8.45565856147914</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>8598</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>8934</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>11008</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>12025</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>13306</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>14111</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>15330</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <v>16568</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>17562</v>
+      </c>
+      <c r="L24" s="4" t="n">
+        <v>104.256803907886</v>
+      </c>
+      <c r="M24" s="4" t="n">
+        <v>9.38723036181124</v>
+      </c>
+      <c r="N24" s="4" t="n">
+        <v>9.14121592579293</v>
+      </c>
+      <c r="O24" s="4" t="n">
+        <v>9.63379933721429</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>444</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>758</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>905</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <v>1184</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>1417</v>
+      </c>
+      <c r="L25" s="4" t="n">
+        <v>598.029556650246</v>
+      </c>
+      <c r="M25" s="4" t="n">
+        <v>33.0810439627229</v>
+      </c>
+      <c r="N25" s="4" t="n">
+        <v>31.5183643083703</v>
+      </c>
+      <c r="O25" s="4" t="n">
+        <v>34.6622911206707</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="J26" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="L26" s="4" t="n">
+        <v>182.142857142857</v>
+      </c>
+      <c r="M26" s="4" t="n">
+        <v>14.8097996568126</v>
+      </c>
+      <c r="N26" s="4" t="n">
+        <v>10.4238533694463</v>
+      </c>
+      <c r="O26" s="4" t="n">
+        <v>19.3699521890136</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>14780</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>16310</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>15615</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>14569</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>15419</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <v>15120</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>14533</v>
+      </c>
+      <c r="J27" s="1" t="n">
+        <v>13458</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>13251</v>
+      </c>
+      <c r="L27" s="4" t="n">
+        <v>-10.3450608930988</v>
+      </c>
+      <c r="M27" s="4" t="n">
+        <v>-1.8199759402309</v>
+      </c>
+      <c r="N27" s="4" t="n">
+        <v>-2.02421994985534</v>
+      </c>
+      <c r="O27" s="4" t="n">
+        <v>-1.6153061558339</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>8341</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>8877</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>9817</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>9938</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>9847</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <v>11233</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>10620</v>
+      </c>
+      <c r="J28" s="1" t="n">
+        <v>11343</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>11341</v>
+      </c>
+      <c r="L28" s="4" t="n">
+        <v>35.966910442393</v>
+      </c>
+      <c r="M28" s="4" t="n">
+        <v>3.73612505736849</v>
+      </c>
+      <c r="N28" s="4" t="n">
+        <v>3.47520824661813</v>
+      </c>
+      <c r="O28" s="4" t="n">
+        <v>3.99769978012776</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>1738</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>1944</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>1934</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>2213</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>2330</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <v>2508</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>2871</v>
+      </c>
+      <c r="J29" s="1" t="n">
+        <v>3025</v>
+      </c>
+      <c r="K29" s="1" t="n">
+        <v>3138</v>
+      </c>
+      <c r="L29" s="4" t="n">
+        <v>80.5523590333717</v>
+      </c>
+      <c r="M29" s="4" t="n">
+        <v>7.97469293774691</v>
+      </c>
+      <c r="N29" s="4" t="n">
+        <v>7.41306406933779</v>
+      </c>
+      <c r="O29" s="4" t="n">
+        <v>8.53925838550569</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>6982</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>7458</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>9246</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>9416</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>10979</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <v>11215</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>12239</v>
+      </c>
+      <c r="J30" s="1" t="n">
+        <v>12594</v>
+      </c>
+      <c r="K30" s="1" t="n">
+        <v>13420</v>
+      </c>
+      <c r="L30" s="4" t="n">
+        <v>92.2085362360355</v>
+      </c>
+      <c r="M30" s="4" t="n">
+        <v>8.23664883096917</v>
+      </c>
+      <c r="N30" s="4" t="n">
+        <v>7.96491740073086</v>
+      </c>
+      <c r="O30" s="4" t="n">
+        <v>8.50906416827617</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>23622</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>23993</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>24901</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>24255</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>25265</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>26806</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>26359</v>
+      </c>
+      <c r="J31" s="1" t="n">
+        <v>26601</v>
+      </c>
+      <c r="K31" s="1" t="n">
+        <v>27352</v>
+      </c>
+      <c r="L31" s="4" t="n">
+        <v>15.7903649140632</v>
+      </c>
+      <c r="M31" s="4" t="n">
+        <v>1.86467340090208</v>
+      </c>
+      <c r="N31" s="4" t="n">
+        <v>1.70315841800344</v>
+      </c>
+      <c r="O31" s="4" t="n">
+        <v>2.02644488605796</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>2932</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>2953</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>3298</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>3424</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>3804</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>3833</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>3747</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>3816</v>
+      </c>
+      <c r="K32" s="1" t="n">
+        <v>4086</v>
+      </c>
+      <c r="L32" s="4" t="n">
+        <v>39.3587994542974</v>
+      </c>
+      <c r="M32" s="4" t="n">
+        <v>4.09376136044051</v>
+      </c>
+      <c r="N32" s="4" t="n">
+        <v>3.65079013161536</v>
+      </c>
+      <c r="O32" s="4" t="n">
+        <v>4.53862571047892</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>20877</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>21260</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>22982</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>22848</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>25350</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>26671</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>27298</v>
+      </c>
+      <c r="J33" s="1" t="n">
+        <v>28350</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v>29399</v>
+      </c>
+      <c r="L33" s="4" t="n">
+        <v>40.8200411936581</v>
+      </c>
+      <c r="M33" s="4" t="n">
+        <v>4.63714497351881</v>
+      </c>
+      <c r="N33" s="4" t="n">
+        <v>4.46913673199816</v>
+      </c>
+      <c r="O33" s="4" t="n">
+        <v>4.80542340746282</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>1514</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>1632</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>1920</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>2037</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>1938</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <v>2103</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>1816</v>
+      </c>
+      <c r="J34" s="1" t="n">
+        <v>1686</v>
+      </c>
+      <c r="K34" s="1" t="n">
+        <v>1739</v>
+      </c>
+      <c r="L34" s="4" t="n">
+        <v>14.8612945838837</v>
+      </c>
+      <c r="M34" s="4" t="n">
+        <v>0.845872871378361</v>
+      </c>
+      <c r="N34" s="4" t="n">
+        <v>0.2495183617643</v>
+      </c>
+      <c r="O34" s="4" t="n">
+        <v>1.44577491625195</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>19797</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>20969</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>23172</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>23360</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>24112</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <v>26194</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v>26105</v>
+      </c>
+      <c r="J35" s="1" t="n">
+        <v>26927</v>
+      </c>
+      <c r="K35" s="1" t="n">
+        <v>27890</v>
+      </c>
+      <c r="L35" s="4" t="n">
+        <v>40.8799313027226</v>
+      </c>
+      <c r="M35" s="4" t="n">
+        <v>4.13858763216548</v>
+      </c>
+      <c r="N35" s="4" t="n">
+        <v>3.96905184102159</v>
+      </c>
+      <c r="O35" s="4" t="n">
+        <v>4.3083998746569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>